<commit_message>
added all graphs for all samples of all wavelengths and their data
</commit_message>
<xml_diff>
--- a/labB/si detector.xlsx
+++ b/labB/si detector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\src\modernoptics\labB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCDD68-AC88-404F-8C89-5795541D70C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5F2D60-5417-417A-BF4D-7F61B44FE69C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31710" yWindow="990" windowWidth="20910" windowHeight="11835" firstSheet="7" activeTab="11" xr2:uid="{8A8EA2A4-E5F9-5742-A087-A152C486879E}"/>
+    <workbookView xWindow="30930" yWindow="2025" windowWidth="20910" windowHeight="11835" firstSheet="12" activeTab="16" xr2:uid="{8A8EA2A4-E5F9-5742-A087-A152C486879E}"/>
   </bookViews>
   <sheets>
     <sheet name="voltage vs wavelength" sheetId="1" r:id="rId1"/>
@@ -14342,7 +14342,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A60"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -15130,8 +15130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBF53D3-95C3-1D4E-88F3-FB4EA162F35F}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B59" sqref="A1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -15569,7 +15569,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B59" sqref="A1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -16004,7 +16004,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B59" sqref="A1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -16439,7 +16439,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B59" sqref="A1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -16874,7 +16874,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B59" sqref="A1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -17308,8 +17308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD48EDF6-9DE9-4141-AFBD-3623728C1154}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -19013,7 +19013,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7069442E-620A-F945-B0A5-99C49A0764D1}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B61" sqref="A2:B61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
   <sheetData>
@@ -19549,8 +19551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B48EDBC-1A29-3145-906D-4ADF0EB12EE1}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -20087,8 +20089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB2ECB9-C5B7-AA4C-857F-17A5709C12A4}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B61" sqref="A2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -20625,8 +20627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0BAECA-7870-2B46-BF3D-C1756A9B4CF7}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B61" sqref="A2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>
@@ -21165,7 +21167,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A61"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18"/>

</xml_diff>